<commit_message>
[0.0.0.0|6] CALC app: - Final starting point for coding; - Designed main GUI form; - Cleaned up unnecessary default project files; - Corrected OOAnalysis.xlsx.
</commit_message>
<xml_diff>
--- a/1_CALC_MVC/OOAnalysis.xlsx
+++ b/1_CALC_MVC/OOAnalysis.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="41">
   <si>
     <t>Object Name</t>
   </si>
@@ -108,9 +108,6 @@
   </si>
   <si>
     <t>Terminates application</t>
-  </si>
-  <si>
-    <t>displays</t>
   </si>
   <si>
     <t>sets value of</t>
@@ -301,21 +298,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -596,10 +593,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H24"/>
+  <dimension ref="A1:H23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -613,18 +610,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="D1" s="6"/>
-      <c r="F1" s="5" t="s">
+      <c r="D1" s="12"/>
+      <c r="F1" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="G1" s="10"/>
-      <c r="H1" s="6"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="12"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
@@ -636,13 +633,13 @@
       <c r="D2" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F2" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="G2" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="H2" s="9" t="s">
+      <c r="H2" s="7" t="s">
         <v>20</v>
       </c>
     </row>
@@ -796,14 +793,14 @@
       <c r="D10" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F10" s="11" t="s">
+      <c r="F10" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="G10" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="H10" s="11" t="s">
-        <v>33</v>
+      <c r="G10" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="H10" s="8" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -837,13 +834,13 @@
         <v>16</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>28</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -856,11 +853,11 @@
       <c r="D13" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F13" s="2" t="s">
-        <v>8</v>
+      <c r="F13" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H13" s="1" t="s">
         <v>5</v>
@@ -868,39 +865,39 @@
     </row>
     <row r="14" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C14" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="F14" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="G14" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="H14" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="D14" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G14" s="1" t="s">
+    </row>
+    <row r="15" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="H14" s="1" t="s">
+      <c r="C15" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="F15" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="G15" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="H15" s="9" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D15" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="F15" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="G15" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="H15" s="12" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -908,133 +905,122 @@
         <v>3</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D16" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="F16" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="G16" s="12" t="s">
+      <c r="D16" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="F16" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="G16" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="H16" s="12" t="s">
-        <v>5</v>
+      <c r="H16" s="9" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C17" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="F17" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="G17" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="H17" s="9" t="s">
         <v>34</v>
-      </c>
-      <c r="D17" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="F17" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="G17" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="H17" s="12" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D18" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="F18" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="G18" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="H18" s="12" t="s">
-        <v>35</v>
+      <c r="D18" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="F18" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="G18" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="H18" s="9" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F19" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="F19" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="G19" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="H19" s="12" t="s">
-        <v>5</v>
+      <c r="G19" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="H19" s="9" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F20" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="G20" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="H20" s="12" t="s">
-        <v>2</v>
+        <v>33</v>
+      </c>
+      <c r="F20" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="G20" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="H20" s="9" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="F21" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="G21" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="H21" s="12" t="s">
-        <v>6</v>
+      <c r="F21" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="G21" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="H21" s="9" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F22" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="G22" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="H22" s="12" t="s">
-        <v>7</v>
+      <c r="F22" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="G22" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="H22" s="10" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F23" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="G23" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="H23" s="13" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F24" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="G24" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="H24" s="12" t="s">
+      <c r="F23" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="G23" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="H23" s="9" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>